<commit_message>
Resolvendo problemas: - Import Excel - Associar Disciplina x Professor - Adicionar Diario OnLine
</commit_message>
<xml_diff>
--- a/war/suporte/excel/ImportarUsuarios.xlsx
+++ b/war/suporte/excel/ImportarUsuarios.xlsx
@@ -22,13 +22,14 @@
     <definedName name="sexo">Auxiliar!$B$2:$B$3</definedName>
     <definedName name="situacaopais">Auxiliar!$D$2:$D$4</definedName>
     <definedName name="TipoPais">Auxiliar!$G$2:$G$6</definedName>
+    <definedName name="unidade_escola">Auxiliar!$H$2:$H$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
   <si>
     <t>Primeiro Nome</t>
   </si>
@@ -298,6 +299,18 @@
   </si>
   <si>
     <t>Padastro</t>
+  </si>
+  <si>
+    <t>Unidade Escola</t>
+  </si>
+  <si>
+    <t>Jaguariúna</t>
+  </si>
+  <si>
+    <t>Santo Antônio de Posse</t>
+  </si>
+  <si>
+    <t>Ambos</t>
   </si>
 </sst>
 </file>
@@ -698,11 +711,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -728,9 +739,10 @@
     <col min="21" max="21" width="13.85546875" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
     <col min="23" max="23" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" s="5" t="s">
         <v>67</v>
       </c>
@@ -800,8 +812,11 @@
       <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="B2" s="1"/>
       <c r="F2" s="6"/>
       <c r="I2" s="1"/>
@@ -810,6 +825,9 @@
       </c>
       <c r="V2" t="s">
         <v>58</v>
+      </c>
+      <c r="X2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +836,7 @@
       <dataRef ref="A1:A6" sheet="Auxiliar"/>
     </dataRefs>
   </dataConsolidate>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
       <formula1>sexo</formula1>
     </dataValidation>
@@ -828,6 +846,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
       <formula1>situacaopais</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2">
+      <formula1>unidade_escola</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -836,11 +857,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -861,9 +880,10 @@
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
     <col min="17" max="17" width="10.85546875" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -918,13 +938,19 @@
       <c r="R1" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="G2" t="s">
         <v>28</v>
       </c>
       <c r="L2" t="s">
         <v>31</v>
+      </c>
+      <c r="S2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -933,12 +959,15 @@
       <dataRef ref="A1:A6" sheet="Auxiliar"/>
     </dataRefs>
   </dataConsolidate>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
       <formula1>sexo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
       <formula1>estados</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+      <formula1>unidade_escola</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -947,11 +976,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -975,9 +1002,10 @@
     <col min="19" max="19" width="13.85546875" customWidth="1"/>
     <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1047,8 +1075,11 @@
       <c r="W1" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="G2" t="s">
         <v>28</v>
       </c>
@@ -1063,6 +1094,9 @@
       </c>
       <c r="W2" t="s">
         <v>62</v>
+      </c>
+      <c r="X2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1071,7 +1105,7 @@
       <dataRef ref="A1:A6" sheet="Auxiliar"/>
     </dataRefs>
   </dataConsolidate>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
       <formula1>sexo</formula1>
     </dataValidation>
@@ -1087,6 +1121,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
       <formula1>TipoPais</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2">
+      <formula1>unidade_escola</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1094,11 +1131,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1119,9 +1154,10 @@
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
     <col min="17" max="17" width="10.85546875" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1176,13 +1212,19 @@
       <c r="R1" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="G2" t="s">
         <v>28</v>
       </c>
       <c r="L2" t="s">
         <v>31</v>
+      </c>
+      <c r="S2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1191,12 +1233,15 @@
       <dataRef ref="A1:A6" sheet="Auxiliar"/>
     </dataRefs>
   </dataConsolidate>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
       <formula1>sexo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
       <formula1>estados</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+      <formula1>unidade_escola</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1205,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1219,9 +1264,10 @@
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -1243,8 +1289,11 @@
       <c r="G1" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1266,8 +1315,11 @@
       <c r="G2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1289,8 +1341,11 @@
       <c r="G3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1303,8 +1358,11 @@
       <c r="G4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1316,7 +1374,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="C6" t="s">
         <v>35</v>
       </c>
@@ -1325,61 +1383,61 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="C7" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="C8" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="C10" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="C11" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="C12" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="C13" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="C14" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="C15" t="s">
         <v>44</v>
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="C16" t="s">
         <v>45</v>
       </c>

</xml_diff>